<commit_message>
Ændret navnene i Risikomatricen samt nogle risici- og konsekvenstal
</commit_message>
<xml_diff>
--- a/Systemarkitektur/Risikomatrix.xlsx
+++ b/Systemarkitektur/Risikomatrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicklas\Dropbox\4. Semester - Gruppe 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mette\Desktop\Projekt-dokumenter\Systemarkitektur\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Navn</t>
   </si>
@@ -38,82 +38,79 @@
     <t>Risiko*kons.</t>
   </si>
   <si>
-    <t>Risikomatrix ver. 1</t>
-  </si>
-  <si>
-    <t>Tilføj en vare til programmet</t>
-  </si>
-  <si>
-    <t>Tilføj en forretning til programmet</t>
-  </si>
-  <si>
-    <t>Tilføj en vare til en forretning</t>
-  </si>
-  <si>
-    <t>Fjern en vare fra programmet</t>
-  </si>
-  <si>
-    <t>Fjern en forretning fra programmet</t>
-  </si>
-  <si>
-    <t>Fjern en vare fra en bestemt forretning</t>
-  </si>
-  <si>
-    <t>Find den billigste forretning for en vare i programmet</t>
-  </si>
-  <si>
-    <t>Finde hvilke forretninger der har en vare</t>
-  </si>
-  <si>
-    <t>Indstillinger for indkøbsseddel</t>
-  </si>
-  <si>
-    <t>Indtast indkøbsseddel</t>
-  </si>
-  <si>
-    <t>Find ud af hvor varerne fra indkøbslisten kan købes billigst</t>
-  </si>
-  <si>
-    <t>Send indkøbsseddel på mail</t>
-  </si>
-  <si>
-    <t>Kunne bestemme afstanden der skal tilbagelægges for at købe varerne fra forslaget</t>
-  </si>
-  <si>
-    <t>Kunne vise en kørselsvejledning mellem de forskellige forretninger, som der skal handles i</t>
-  </si>
-  <si>
-    <t>Autofuldførelse</t>
-  </si>
-  <si>
-    <t>Bekræftelse af oprettelse/sletning af vare</t>
-  </si>
-  <si>
-    <t>Ugentlig madplan</t>
-  </si>
-  <si>
-    <t>Find åbningstider for en forretning</t>
-  </si>
-  <si>
-    <t>Se en sammenligning af hvad det koster at købe alle varer i en enkelt forretning eller købe varerne der hvor det er billigst</t>
-  </si>
-  <si>
-    <t>Juster hvor varer skal købes efter programmet er kommet med et forslag</t>
-  </si>
-  <si>
-    <t>Tilføj en opskrifter til programmet</t>
-  </si>
-  <si>
-    <t>Fjern en opskrift fra programmet</t>
-  </si>
-  <si>
-    <t>Find en opskrift I programmet</t>
-  </si>
-  <si>
-    <t>Ændre en opskrift</t>
-  </si>
-  <si>
-    <t>Generer indkøbslist fra opskrifter</t>
+    <t>Risikomatrix ver. 2</t>
+  </si>
+  <si>
+    <t>Forretningsmanageren kan tilføje en vare til sin forretning i Pristjek220</t>
+  </si>
+  <si>
+    <t>Administratoren kan tilføje en forretning med tilhørende forretningsmanager til Pristjek220</t>
+  </si>
+  <si>
+    <t>Administratoren kan fjerne en vare fra Pristjek220</t>
+  </si>
+  <si>
+    <t>Administratoren kan fjerne en forretning fra Pristjek220</t>
+  </si>
+  <si>
+    <t>Forretningsmanageren kan fjerne en vare fra sin forretning fra Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan finde den billigste forretning for en vare i Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan i Pristjek220 finde hvilke forretninger der har en vare</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan finde åbningstider for en forretning i Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan indtaste en indkøbsliste i Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan sætte indstillinger for en indkøbsliste</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan gennem Pristjek220 kunne finde ud af hvor varerne fra indkøbslisten kan købes billigst</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan se en sammenligning af hvad det koster at købe alle varer i en enkelt forretning eller købe varerne der hvor det er billigst</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan justere hvor varer skal købes efter Pristjek220 er kommet med et forslag</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan få tilsendt sin indkøbsliste på mail</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan få vist afstanden der skal tilbagelægges for at købe varerne fra forslaget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forbrugeren kan få vist en kørselsvejledning mellem de forskellige forretninger, som der skal handles i </t>
+  </si>
+  <si>
+    <t>Forbrugeren vil blive foreslået varer når han begynder at indtaste bogstaver i søgefeltet i Pristjek220</t>
+  </si>
+  <si>
+    <t>Forretningsmanageren vil blive bedt om at bekræfte oprettelsen eller sletningen af varer</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan tilføje en opskrift til Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan fjerne en opskrift fra Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan finde en opskrift i Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan ændre en opskrift i Pristjek220</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan gennem Pristjek220 generere en indkøbsliste ud fra en eller flere opskrifter</t>
+  </si>
+  <si>
+    <t>Forbrugeren kan oprette en ugentlig madplan</t>
   </si>
 </sst>
 </file>
@@ -228,12 +225,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -518,20 +521,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:F28"/>
+  <dimension ref="C2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="110" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
@@ -539,8 +542,8 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -553,8 +556,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2">
@@ -568,8 +571,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2">
@@ -583,23 +586,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2">
@@ -613,305 +616,305 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
         <v>2</v>
       </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
         <v>2</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F21" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
-        <f t="shared" si="0"/>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="2">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="2">
-        <v>3</v>
-      </c>
-      <c r="E17" s="2">
-        <v>3</v>
-      </c>
-      <c r="F17" s="2">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="2">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2">
-        <v>4</v>
-      </c>
-      <c r="E21" s="2">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="2">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="2">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="D27" s="2">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1</v>
+      </c>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Ændret så det er administratoren og ikke forbrugeren der kan fjerne opskrifter.
</commit_message>
<xml_diff>
--- a/Systemarkitektur/Risikomatrix.xlsx
+++ b/Systemarkitektur/Risikomatrix.xlsx
@@ -98,9 +98,6 @@
     <t>Forbrugeren kan tilføje en opskrift til Pristjek220</t>
   </si>
   <si>
-    <t>Forbrugeren kan fjerne en opskrift fra Pristjek220</t>
-  </si>
-  <si>
     <t>Forbrugeren kan finde en opskrift i Pristjek220</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>Forbrugeren kan oprette en ugentlig madplan</t>
+  </si>
+  <si>
+    <t>Administratoren kan fjerne en opskrift fra Pristjek220</t>
   </si>
 </sst>
 </file>
@@ -229,14 +229,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -523,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,15 +535,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -557,7 +557,7 @@
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2">
@@ -572,7 +572,7 @@
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2">
@@ -587,7 +587,7 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2">
@@ -602,7 +602,7 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2">
@@ -617,7 +617,7 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2">
@@ -632,7 +632,7 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2">
@@ -647,7 +647,7 @@
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2">
@@ -662,7 +662,7 @@
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2">
@@ -677,7 +677,7 @@
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2">
@@ -692,7 +692,7 @@
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="2">
@@ -707,7 +707,7 @@
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="2">
@@ -722,7 +722,7 @@
       </c>
     </row>
     <row r="15" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="2">
@@ -737,7 +737,7 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="2">
@@ -752,7 +752,7 @@
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="2">
@@ -767,7 +767,7 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="2">
@@ -782,7 +782,7 @@
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="2">
@@ -797,7 +797,7 @@
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="2">
@@ -812,7 +812,7 @@
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="2">
@@ -827,7 +827,7 @@
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="2">
@@ -842,68 +842,68 @@
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="2">
-        <v>3</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="2">
-        <v>3</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="D25" s="2">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="2">
-        <v>4</v>
-      </c>
-      <c r="E25" s="2">
-        <v>1</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="2">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D26" s="2">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="D27" s="2">
         <v>4</v>

</xml_diff>